<commit_message>
Adding video and Jenkins output
</commit_message>
<xml_diff>
--- a/src/test/java/Utils/AdactinTestData.xlsx
+++ b/src/test/java/Utils/AdactinTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\girit\workspace\adactHotel\src\test\java\Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A4E5A1-68D0-48DF-A568-3B20890BB95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4B3F02-AB10-4F47-80E3-0B7A42129331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{D8210BAF-AA6E-4505-A6F9-573B3C439A6A}"/>
   </bookViews>
@@ -403,13 +403,13 @@
     <t>Please Select your Credit Card Expiry Year</t>
   </si>
   <si>
-    <t>9686GX138E</t>
-  </si>
-  <si>
-    <t>59929LMZ32</t>
-  </si>
-  <si>
-    <t>9BDM8WT052,HM7GMFNY97</t>
+    <t>343H6ST69D</t>
+  </si>
+  <si>
+    <t>99ICOJ4827</t>
+  </si>
+  <si>
+    <t>J675XG04RX,0G1D9MIP8G</t>
   </si>
 </sst>
 </file>
@@ -2123,7 +2123,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>